<commit_message>
Table edit without having to press enter
</commit_message>
<xml_diff>
--- a/OptimizerGATestSuit/out/TestSuiteApp/results/ExcelResults.xlsx
+++ b/OptimizerGATestSuit/out/TestSuiteApp/results/ExcelResults.xlsx
@@ -13,9 +13,9 @@
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Genetic Population" r:id="rId8" sheetId="10"/>
-    <sheet name="GA Results" r:id="rId6" sheetId="11"/>
-    <sheet name="Greedy Results" r:id="rId7" sheetId="12"/>
+    <sheet name="Genetic Population" r:id="rId8" sheetId="13"/>
+    <sheet name="GA Results" r:id="rId6" sheetId="14"/>
+    <sheet name="Greedy Results" r:id="rId7" sheetId="15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="191">
   <si>
     <t xml:space="preserve">Test cases array = </t>
   </si>
@@ -537,6 +537,81 @@
   </si>
   <si>
     <t>Greedy minimization % = 17.1875</t>
+  </si>
+  <si>
+    <t>[2, 3, 2, 3, 32, 25, 56, 4, 3, 4]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 1, 1, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 1, 1, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0, 1, 0, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 1, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 1, 1, 0, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 1, 0, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 1, 1, 0, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 1, 0, 1, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1, 0, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 1, 1, 0, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 1, 1, 0, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>Genes=[0, 0, 1, 0, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>Statements covered = 97</t>
+  </si>
+  <si>
+    <t>GA % of coverage = 194.0%</t>
+  </si>
+  <si>
+    <t>Genes=[0, 0, 0, 0, 0, 0, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>Total test cases = 1</t>
+  </si>
+  <si>
+    <t>Statements covered = 56</t>
+  </si>
+  <si>
+    <t>Greedy % of coverage = 112.0</t>
+  </si>
+  <si>
+    <t>Greedy minimization % = 42.26804</t>
   </si>
 </sst>
 </file>
@@ -853,7 +928,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A2:B104"/>
   <sheetViews>
@@ -866,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4">
@@ -879,802 +954,802 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B5" t="n">
-        <v>64.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B6" t="n">
-        <v>64.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B7" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B8" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B9" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B10" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B11" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B12" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="B14" t="n">
-        <v>64.0</v>
+        <v>117.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B15" t="n">
-        <v>64.0</v>
+        <v>106.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B16" t="n">
-        <v>64.0</v>
+        <v>103.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="B17" t="n">
-        <v>64.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="B18" t="n">
-        <v>64.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="B19" t="n">
-        <v>64.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B20" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B21" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B22" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B23" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B24" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B25" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B26" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B27" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B28" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B29" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B30" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B31" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B32" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B33" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B34" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B35" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B36" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B37" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B38" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B39" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B40" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B41" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B42" t="n">
-        <v>64.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
-        <v>63.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B44" t="n">
-        <v>63.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="B45" t="n">
-        <v>63.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B46" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B47" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B48" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B49" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B50" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B51" t="n">
-        <v>62.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B52" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B53" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B54" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B55" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="B56" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B57" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="B58" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B59" t="n">
-        <v>60.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B60" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B61" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B62" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B63" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B64" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B65" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B66" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B67" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B68" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B69" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B70" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B71" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B72" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B73" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B74" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B75" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B76" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B77" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B78" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="B79" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B80" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B81" t="n">
-        <v>60.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="B82" t="n">
-        <v>60.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="B83" t="n">
-        <v>60.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="B84" t="n">
-        <v>60.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
       <c r="B85" t="n">
-        <v>60.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="B86" t="n">
-        <v>60.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="B87" t="n">
-        <v>59.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="B88" t="n">
-        <v>57.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B89" t="n">
-        <v>57.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B90" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B91" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B92" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B93" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="B94" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B95" t="n">
-        <v>56.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B96" t="n">
-        <v>56.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="B97" t="n">
-        <v>56.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="B98" t="n">
-        <v>56.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="B99" t="n">
-        <v>56.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="B100" t="n">
-        <v>56.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="B101" t="n">
-        <v>56.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="B102" t="n">
-        <v>55.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B103" t="n">
-        <v>64.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="B104" t="n">
-        <v>55.0</v>
+        <v>70.0</v>
       </c>
     </row>
   </sheetData>
@@ -1682,9 +1757,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B15"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1692,7 +1767,7 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
@@ -1708,7 +1783,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
@@ -1716,7 +1791,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" t="n">
-        <v>8.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="7">
@@ -1724,7 +1799,7 @@
         <v>3.0</v>
       </c>
       <c r="B7" t="n">
-        <v>7.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="8">
@@ -1732,7 +1807,7 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
@@ -1740,36 +1815,20 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="n">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B10" t="n">
-        <v>16.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B11" t="n">
-        <v>6.0</v>
+      <c r="A11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1777,9 +1836,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B14"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1787,7 +1846,7 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4">
@@ -1803,57 +1862,25 @@
         <v>1.0</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>8.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>12.0</v>
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>165</v>
+      <c r="A9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>